<commit_message>
test suite 2company - appForm appRea AppFile
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\regression\channelingBU\atchbu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\regression\repo\atchbu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71ED99AB-FFF7-4990-84DB-D70E18754AE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739B99BE-2A44-4EC4-A2B9-7B0637978A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Testing" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="112">
   <si>
     <t>Nama_Debitur</t>
   </si>
@@ -156,220 +156,230 @@
     <t>INDUSTRI KOMPONEN DAN PAPAN ELEKTRONIK</t>
   </si>
   <si>
+    <t>P02</t>
+  </si>
+  <si>
+    <t>3512</t>
+  </si>
+  <si>
+    <t>Kab. Kuantan Singingi</t>
+  </si>
+  <si>
+    <t>200000</t>
+  </si>
+  <si>
+    <t>300000</t>
+  </si>
+  <si>
+    <t>P03</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>451000</t>
+  </si>
+  <si>
+    <t>S1500303L</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>400000</t>
+  </si>
+  <si>
+    <t>500000</t>
+  </si>
+  <si>
+    <t>600000</t>
+  </si>
+  <si>
+    <t>P04</t>
+  </si>
+  <si>
+    <t>P05</t>
+  </si>
+  <si>
+    <t>P06</t>
+  </si>
+  <si>
+    <t>Dengan Perjanjian Kredit / Pembiayaan - Kredit / Pembiayaan kepada pihak ketiga melalui lembaga lain secara channeling</t>
+  </si>
+  <si>
+    <t>Dengan Perjanjian Kredit / Pembiayaan - Kredit / Pembiayaan kepada UMKM melalui lembaga lain secara executing</t>
+  </si>
+  <si>
+    <t>Dengan Perjanjian Kredit / Pembiayaan - Kredit / Pembiayaan kepada Non-UMKM melalui lembaga lain secara executing</t>
+  </si>
+  <si>
+    <t>Dengan Perjanjian Kredit / Pembiayaan - Kartu Kredit / Kartu Pembiayaan Syariah</t>
+  </si>
+  <si>
+    <t>Dengan Perjanjian Kredit / Pembiayaan - Surat berharga dengan Note Purchase Agreement</t>
+  </si>
+  <si>
+    <t>Konsumsi</t>
+  </si>
+  <si>
+    <t>Industri Pengolahan</t>
+  </si>
+  <si>
+    <t>Konstruksi</t>
+  </si>
+  <si>
+    <t>Penyediaan Akomodasi dan Penyediaan Makan Minum</t>
+  </si>
+  <si>
+    <t>Perantara Keuangan</t>
+  </si>
+  <si>
+    <t>Administrasi Pemerintahan, Pertahanan dan Jaminan Sosial</t>
+  </si>
+  <si>
+    <t>Commanditer Venpotschap (CV)</t>
+  </si>
+  <si>
+    <t>Debitur Kelompok</t>
+  </si>
+  <si>
+    <t>Lembaga Non Profit Melayani Rumah Tangga - Swasta Pengendalian Asing - Lembaga Wakaf</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Deskripsi</t>
+  </si>
+  <si>
+    <t>Dati II</t>
+  </si>
+  <si>
+    <t>0113</t>
+  </si>
+  <si>
+    <t>0111</t>
+  </si>
+  <si>
+    <t>Kab. Tasikmalaya</t>
+  </si>
+  <si>
+    <t>Kab. Bandung</t>
+  </si>
+  <si>
+    <t>Sandi Jabatan</t>
+  </si>
+  <si>
+    <t>Bentuk Pengurus</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>PEMILIK - Ketua</t>
+  </si>
+  <si>
+    <t>PEMILIK - Sekretaris</t>
+  </si>
+  <si>
+    <t>PEMILIK - Direktur Utama / Pres. Dir</t>
+  </si>
+  <si>
+    <t>Badan Usaha</t>
+  </si>
+  <si>
+    <t>Kab. Kepulauan Meranti</t>
+  </si>
+  <si>
+    <t>3513</t>
+  </si>
+  <si>
+    <t>Modal Kerja</t>
+  </si>
+  <si>
+    <t>S1500302L</t>
+  </si>
+  <si>
+    <t>Lembaga Non Profit Melayani Rumah Tangga - Swasta Pengendalian Asing - Lembaga Pendidikan</t>
+  </si>
+  <si>
+    <t>Badan Usaha Milik Desa (BUMDes)</t>
+  </si>
+  <si>
+    <t>550000</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>S1500301L</t>
+  </si>
+  <si>
+    <t>Lembaga Non Profit Melayani Rumah Tangga - Swasta Pengendalian Asing - BAZIS</t>
+  </si>
+  <si>
+    <t>PEMILIK - Masyarakat</t>
+  </si>
+  <si>
+    <t>PEMILIK - Ketua Umum</t>
+  </si>
+  <si>
+    <t>PEMILIK - Bendahara</t>
+  </si>
+  <si>
+    <t>Kab. Siak</t>
+  </si>
+  <si>
+    <t>3511</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>L000002</t>
+  </si>
+  <si>
+    <t>24BL002</t>
+  </si>
+  <si>
+    <t>NEW KOMUNAL</t>
+  </si>
+  <si>
     <t>8</t>
   </si>
   <si>
-    <t>P02</t>
-  </si>
-  <si>
-    <t>3512</t>
-  </si>
-  <si>
-    <t>Kab. Kuantan Singingi</t>
-  </si>
-  <si>
-    <t>200000</t>
-  </si>
-  <si>
-    <t>300000</t>
-  </si>
-  <si>
-    <t>P03</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>451000</t>
-  </si>
-  <si>
-    <t>S1500303L</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>400000</t>
-  </si>
-  <si>
-    <t>500000</t>
-  </si>
-  <si>
-    <t>600000</t>
-  </si>
-  <si>
-    <t>P04</t>
-  </si>
-  <si>
-    <t>P05</t>
-  </si>
-  <si>
-    <t>P06</t>
-  </si>
-  <si>
-    <t>Dengan Perjanjian Kredit / Pembiayaan - Kredit / Pembiayaan kepada pihak ketiga melalui lembaga lain secara channeling</t>
-  </si>
-  <si>
-    <t>Dengan Perjanjian Kredit / Pembiayaan - Kredit / Pembiayaan kepada UMKM melalui lembaga lain secara executing</t>
-  </si>
-  <si>
-    <t>Dengan Perjanjian Kredit / Pembiayaan - Kredit / Pembiayaan kepada Non-UMKM melalui lembaga lain secara executing</t>
-  </si>
-  <si>
-    <t>Dengan Perjanjian Kredit / Pembiayaan - Kartu Kredit / Kartu Pembiayaan Syariah</t>
-  </si>
-  <si>
-    <t>Dengan Perjanjian Kredit / Pembiayaan - Surat berharga dengan Note Purchase Agreement</t>
-  </si>
-  <si>
-    <t>Konsumsi</t>
-  </si>
-  <si>
-    <t>Industri Pengolahan</t>
-  </si>
-  <si>
-    <t>Konstruksi</t>
-  </si>
-  <si>
-    <t>Penyediaan Akomodasi dan Penyediaan Makan Minum</t>
-  </si>
-  <si>
-    <t>Perantara Keuangan</t>
-  </si>
-  <si>
-    <t>Administrasi Pemerintahan, Pertahanan dan Jaminan Sosial</t>
-  </si>
-  <si>
-    <t>Commanditer Venpotschap (CV)</t>
-  </si>
-  <si>
-    <t>Debitur Kelompok</t>
-  </si>
-  <si>
-    <t>Lembaga Non Profit Melayani Rumah Tangga - Swasta Pengendalian Asing - Lembaga Wakaf</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Deskripsi</t>
-  </si>
-  <si>
-    <t>Dati II</t>
-  </si>
-  <si>
-    <t>0113</t>
-  </si>
-  <si>
-    <t>0111</t>
-  </si>
-  <si>
-    <t>Kab. Tasikmalaya</t>
-  </si>
-  <si>
-    <t>Kab. Bandung</t>
-  </si>
-  <si>
-    <t>Sandi Jabatan</t>
-  </si>
-  <si>
-    <t>Bentuk Pengurus</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>PEMILIK - Ketua</t>
-  </si>
-  <si>
-    <t>PEMILIK - Sekretaris</t>
-  </si>
-  <si>
-    <t>PEMILIK - Direktur Utama / Pres. Dir</t>
-  </si>
-  <si>
-    <t>Badan Usaha</t>
-  </si>
-  <si>
-    <t>Kab. Kepulauan Meranti</t>
-  </si>
-  <si>
-    <t>3513</t>
-  </si>
-  <si>
-    <t>Modal Kerja</t>
-  </si>
-  <si>
-    <t>S1500302L</t>
-  </si>
-  <si>
-    <t>Lembaga Non Profit Melayani Rumah Tangga - Swasta Pengendalian Asing - Lembaga Pendidikan</t>
-  </si>
-  <si>
-    <t>Badan Usaha Milik Desa (BUMDes)</t>
-  </si>
-  <si>
-    <t>550000</t>
-  </si>
-  <si>
-    <t>18</t>
-  </si>
-  <si>
-    <t>S1500301L</t>
-  </si>
-  <si>
-    <t>Lembaga Non Profit Melayani Rumah Tangga - Swasta Pengendalian Asing - BAZIS</t>
-  </si>
-  <si>
-    <t>PEMILIK - Masyarakat</t>
-  </si>
-  <si>
-    <t>PEMILIK - Ketua Umum</t>
-  </si>
-  <si>
-    <t>PEMILIK - Bendahara</t>
-  </si>
-  <si>
-    <t>Kab. Siak</t>
-  </si>
-  <si>
-    <t>3511</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>13</t>
-  </si>
-  <si>
-    <t>NEW KOMUNAL</t>
-  </si>
-  <si>
-    <t>L000002</t>
-  </si>
-  <si>
-    <t>24BL002</t>
-  </si>
-  <si>
-    <t>092830</t>
-  </si>
-  <si>
-    <t>realizationForm</t>
+    <t>163242</t>
+  </si>
+  <si>
+    <t>validationApprovalFile</t>
+  </si>
+  <si>
+    <t>163750</t>
+  </si>
+  <si>
+    <t>163908</t>
+  </si>
+  <si>
+    <t>163909</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -504,11 +514,11 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -793,22 +803,22 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="3" width="24.85546875" style="2" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="20.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="23.28515625" style="2" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.7109375" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="15.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="21.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="17.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="21.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="16384" width="9.140625" style="2" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="13.85546875" collapsed="true"/>
+    <col min="2" max="3" customWidth="true" style="2" width="24.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="2" width="20.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="2" width="23.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="12.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="2" width="15.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="2" width="21.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="2" width="17.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="2" width="21.85546875" collapsed="true"/>
+    <col min="12" max="16384" style="2" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -857,16 +867,16 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" t="s">
         <v>104</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
@@ -875,7 +885,7 @@
         <v>108</v>
       </c>
       <c r="I2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>14</v>
@@ -887,13 +897,13 @@
       <formula1>"SummerCORP,RainnyCORP,SunnyCORP,CloudyCORP,SnowyCORP,StormCORP,FoggyCORP,OtoCORP,AutoCORP"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{CF038CEC-345B-41BF-B448-317F71DA7E05}">
-      <formula1>"L000030,L000001,L000002,L000053"</formula1>
+      <formula1>"L000030,L000001,L000002,L000053,L000060"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{8B1A4411-E596-43F9-B4F1-D6969A139641}">
-      <formula1>"AKSELERAN,NEW KOMUNAL"</formula1>
+      <formula1>"AKSELERAN,NEW KOMUNAL,PT Tes Pending"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{D7BE5674-80E4-483C-8297-552124B3A817}">
-      <formula1>"24BL008,24BL010,24BL001,24BL002"</formula1>
+      <formula1>"24BL008,24BL010,24BL001,24BL002,24BL001"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{85650A16-C576-480A-9F93-6FAB323B5478}">
       <formula1>"UAT,E2E"</formula1>
@@ -917,42 +927,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5" collapsed="1"/>
-    <col min="2" max="2" width="11.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="99.28515625" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="2.42578125" style="4" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.140625" style="5" collapsed="1"/>
-    <col min="6" max="6" width="11.85546875" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="111.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="2.5703125" style="4" customWidth="1" collapsed="1"/>
-    <col min="9" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" style="5" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="11.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="99.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="4" width="2.42578125" collapsed="true"/>
+    <col min="5" max="5" style="5" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="11.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="5" width="111.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="4" width="2.5703125" collapsed="true"/>
+    <col min="9" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="17"/>
+      <c r="C1" s="16"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="17"/>
+      <c r="G1" s="16"/>
     </row>
     <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="16"/>
+      <c r="A2" s="17"/>
       <c r="B2" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="16"/>
+      <c r="E2" s="17"/>
       <c r="F2" s="15" t="s">
         <v>27</v>
       </c>
@@ -984,20 +994,20 @@
     <row r="4" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D4" s="7"/>
       <c r="F4" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H4" s="7"/>
     </row>
     <row r="5" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D5" s="7"/>
       <c r="F5" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H5" s="7"/>
     </row>
@@ -1008,10 +1018,10 @@
       <c r="C6" s="15"/>
       <c r="D6" s="6"/>
       <c r="F6" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H6" s="7"/>
     </row>
@@ -1024,20 +1034,20 @@
       </c>
       <c r="D7" s="7"/>
       <c r="F7" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H7" s="7"/>
     </row>
     <row r="8" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D8" s="7"/>
       <c r="F8" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H8" s="7"/>
     </row>
@@ -1076,10 +1086,10 @@
     <row r="12" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D12" s="7"/>
       <c r="F12" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H12" s="7"/>
     </row>
@@ -1152,10 +1162,10 @@
     <row r="20" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D20" s="7"/>
       <c r="F20" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="9" t="s">
         <v>41</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="H20" s="7"/>
     </row>
@@ -1228,20 +1238,20 @@
     <row r="28" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D28" s="7"/>
       <c r="F28" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H28" s="7"/>
     </row>
     <row r="29" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D29" s="7"/>
       <c r="F29" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H29" s="7"/>
     </row>
@@ -1252,10 +1262,10 @@
       <c r="C30" s="15"/>
       <c r="D30" s="6"/>
       <c r="F30" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G30" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H30" s="7"/>
     </row>
@@ -1268,20 +1278,20 @@
       </c>
       <c r="D31" s="7"/>
       <c r="F31" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G31" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H31" s="7"/>
     </row>
     <row r="32" spans="2:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D32" s="7"/>
       <c r="F32" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G32" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H32" s="7"/>
     </row>
@@ -1301,18 +1311,18 @@
     </row>
     <row r="36" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F36" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G36" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F37" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G37" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="6:7" x14ac:dyDescent="0.25">
@@ -1343,7 +1353,7 @@
     </row>
     <row r="44" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F44" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G44" s="9" t="s">
         <v>22</v>
@@ -1419,10 +1429,10 @@
     </row>
     <row r="60" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F60" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G60" s="9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="61" spans="6:7" x14ac:dyDescent="0.25">
@@ -1455,15 +1465,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F34:G34"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="A1:A2"/>
@@ -1475,6 +1476,15 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B22:C22"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F34:G34"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1492,13 +1502,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="18.42578125" style="5" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="116.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="27.5703125" style="5" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18.140625" style="5" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="116.5703125" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="16384" width="9.140625" style="5" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="5" width="27.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="5" width="18.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="5" width="116.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="5" width="27.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="5" width="18.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="5" width="116.5703125" collapsed="true"/>
+    <col min="7" max="16384" style="5" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -1506,24 +1516,24 @@
         <v>34</v>
       </c>
       <c r="B1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="12" t="s">
         <v>70</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>71</v>
       </c>
       <c r="D1" s="12" t="s">
         <v>15</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F1" s="12" t="s">
         <v>70</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>36</v>
@@ -1532,7 +1542,7 @@
         <v>35</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>36</v>
@@ -1543,72 +1553,72 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>42</v>
-      </c>
       <c r="E3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="F6" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="F7" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1616,7 +1626,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="13" t="s">
         <v>20</v>
@@ -1625,7 +1635,7 @@
         <v>30</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F8" s="13" t="s">
         <v>20</v>
@@ -1633,72 +1643,72 @@
     </row>
     <row r="9" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1723,72 +1733,72 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1796,30 +1806,30 @@
         <v>28</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>28</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>19</v>
@@ -1827,16 +1837,16 @@
     </row>
     <row r="22" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1864,13 +1874,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C27" s="5" t="s">
         <v>22</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F27" s="5" t="s">
         <v>22</v>
@@ -1881,7 +1891,7 @@
         <v>23</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C32" s="13" t="s">
         <v>23</v>
@@ -1890,7 +1900,7 @@
         <v>23</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F32" s="13" t="s">
         <v>23</v>
@@ -1923,44 +1933,44 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C40" s="5" t="s">
-        <v>90</v>
-      </c>
       <c r="E40" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F40" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B41" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C41" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="E41" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="F41" s="5" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1968,47 +1978,47 @@
         <v>31</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C44" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D44" s="13" t="s">
         <v>31</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F44" s="13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B45" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C45" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F45" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="46" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C46" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F46" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
@@ -2019,7 +2029,7 @@
         <v>21</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F47" s="13" t="s">
         <v>21</v>
@@ -2029,112 +2039,112 @@
     <row r="49" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B51" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="56" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B56" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="B56" s="13" t="s">
-        <v>79</v>
-      </c>
       <c r="C56" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D56" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="E56" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="E56" s="13" t="s">
-        <v>79</v>
-      </c>
       <c r="F56" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated scenario appForm, reaForm, validateFile and pengurusForm
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\regression\repo\atchbu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\channeling\atchbu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{739B99BE-2A44-4EC4-A2B9-7B0637978A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D353779-A6A4-4E93-8DA6-78D87DF72FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Testing" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="127">
   <si>
     <t>Nama_Debitur</t>
   </si>
@@ -348,31 +348,76 @@
     <t>13</t>
   </si>
   <si>
-    <t>L000002</t>
-  </si>
-  <si>
-    <t>24BL002</t>
-  </si>
-  <si>
-    <t>NEW KOMUNAL</t>
+    <t>AKSELERAN</t>
+  </si>
+  <si>
+    <t>Jenis Kelamin Pengurus</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Perorangan</t>
+  </si>
+  <si>
+    <t>Pria/Laki-laki</t>
+  </si>
+  <si>
+    <t>Wanita/Perempuan</t>
+  </si>
+  <si>
+    <t>Masyarakat</t>
+  </si>
+  <si>
+    <t>Laki-laki</t>
+  </si>
+  <si>
+    <t>Perempuan</t>
+  </si>
+  <si>
+    <t>L000001</t>
+  </si>
+  <si>
+    <t>24BL001</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>163242</t>
-  </si>
-  <si>
-    <t>validationApprovalFile</t>
-  </si>
-  <si>
-    <t>163750</t>
-  </si>
-  <si>
-    <t>163908</t>
-  </si>
-  <si>
-    <t>163909</t>
+    <t>121144</t>
+  </si>
+  <si>
+    <t>approvalForm</t>
+  </si>
+  <si>
+    <t>132444</t>
+  </si>
+  <si>
+    <t>132445</t>
+  </si>
+  <si>
+    <t>133908</t>
+  </si>
+  <si>
+    <t>133909</t>
+  </si>
+  <si>
+    <t>152541</t>
+  </si>
+  <si>
+    <t>152542</t>
+  </si>
+  <si>
+    <t>154541</t>
   </si>
 </sst>
 </file>
@@ -514,11 +559,11 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -803,10 +848,10 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="13.85546875" collapsed="true"/>
     <col min="2" max="3" customWidth="true" style="2" width="24.85546875" collapsed="true"/>
@@ -867,25 +912,25 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="I2" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>14</v>
@@ -897,19 +942,19 @@
       <formula1>"SummerCORP,RainnyCORP,SunnyCORP,CloudyCORP,SnowyCORP,StormCORP,FoggyCORP,OtoCORP,AutoCORP"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{CF038CEC-345B-41BF-B448-317F71DA7E05}">
-      <formula1>"L000030,L000001,L000002,L000053,L000060"</formula1>
+      <formula1>"L000030,L000001,L000002,L000053"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{8B1A4411-E596-43F9-B4F1-D6969A139641}">
-      <formula1>"AKSELERAN,NEW KOMUNAL,PT Tes Pending"</formula1>
+      <formula1>"AKSELERAN,NEW KOMUNAL"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{D7BE5674-80E4-483C-8297-552124B3A817}">
-      <formula1>"24BL008,24BL010,24BL001,24BL002,24BL001"</formula1>
+      <formula1>"24BL008,24BL010,24BL001,24BL002"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2" xr:uid="{85650A16-C576-480A-9F93-6FAB323B5478}">
       <formula1>"UAT,E2E"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{522E0E79-AC07-422F-B8D2-DC41E42871EC}">
-      <formula1>"approvalForm,realizationForm,validationApprovalFile,validationRealizationFile"</formula1>
+      <formula1>"approvalForm,repaymentForm,realizationForm,validationApprovalFile,validationRealizationFile"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -921,11 +966,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4783489F-3DBC-42F1-8026-4170A2B0020B}">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F28" sqref="F28:G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="5" width="9.140625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="11.85546875" collapsed="true"/>
@@ -939,30 +984,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="16"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="17" t="s">
+      <c r="E1" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="16"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
+      <c r="A2" s="16"/>
       <c r="B2" s="15" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="15"/>
       <c r="D2" s="6"/>
-      <c r="E2" s="17"/>
+      <c r="E2" s="16"/>
       <c r="F2" s="15" t="s">
         <v>27</v>
       </c>
@@ -1465,6 +1510,15 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="F50:G50"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="F34:G34"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="A1:A2"/>
@@ -1476,15 +1530,6 @@
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="F50:G50"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="F34:G34"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1494,13 +1539,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E3C999F-07B3-4113-999F-F6E43F98FC0B}">
-  <dimension ref="A1:F61"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
-    <sheetView topLeftCell="B28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="5" width="27.5703125" collapsed="true"/>
     <col min="2" max="2" customWidth="true" style="5" width="18.42578125" collapsed="true"/>
@@ -2147,11 +2192,86 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E57" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
     <row r="58" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="59" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="60" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E62" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
BU week 1 march
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\project\channeling\atchbu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D353779-A6A4-4E93-8DA6-78D87DF72FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BC2BFA-FE0B-4EBC-B57A-AC9BAF13268D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="147">
   <si>
     <t>Nama_Debitur</t>
   </si>
@@ -348,76 +348,136 @@
     <t>13</t>
   </si>
   <si>
+    <t>Jenis Kelamin Pengurus</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Perorangan</t>
+  </si>
+  <si>
+    <t>Pria/Laki-laki</t>
+  </si>
+  <si>
+    <t>Wanita/Perempuan</t>
+  </si>
+  <si>
+    <t>Masyarakat</t>
+  </si>
+  <si>
+    <t>Laki-laki</t>
+  </si>
+  <si>
+    <t>Perempuan</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>realizationForm</t>
+  </si>
+  <si>
+    <t>153554</t>
+  </si>
+  <si>
     <t>AKSELERAN</t>
   </si>
   <si>
-    <t>Jenis Kelamin Pengurus</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>Perorangan</t>
-  </si>
-  <si>
-    <t>Pria/Laki-laki</t>
-  </si>
-  <si>
-    <t>Wanita/Perempuan</t>
-  </si>
-  <si>
-    <t>Masyarakat</t>
-  </si>
-  <si>
-    <t>Laki-laki</t>
-  </si>
-  <si>
-    <t>Perempuan</t>
-  </si>
-  <si>
     <t>L000001</t>
   </si>
   <si>
     <t>24BL001</t>
   </si>
   <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>121144</t>
-  </si>
-  <si>
-    <t>approvalForm</t>
-  </si>
-  <si>
-    <t>132444</t>
-  </si>
-  <si>
-    <t>132445</t>
-  </si>
-  <si>
-    <t>133908</t>
-  </si>
-  <si>
-    <t>133909</t>
-  </si>
-  <si>
-    <t>152541</t>
-  </si>
-  <si>
-    <t>152542</t>
-  </si>
-  <si>
-    <t>154541</t>
+    <t>154755</t>
+  </si>
+  <si>
+    <t>154756</t>
+  </si>
+  <si>
+    <t>161048</t>
+  </si>
+  <si>
+    <t>174852</t>
+  </si>
+  <si>
+    <t>174853</t>
+  </si>
+  <si>
+    <t>183730</t>
+  </si>
+  <si>
+    <t>005538</t>
+  </si>
+  <si>
+    <t>005539</t>
+  </si>
+  <si>
+    <t>010916</t>
+  </si>
+  <si>
+    <t>105513</t>
+  </si>
+  <si>
+    <t>105514</t>
+  </si>
+  <si>
+    <t>105539</t>
+  </si>
+  <si>
+    <t>105540</t>
+  </si>
+  <si>
+    <t>105845</t>
+  </si>
+  <si>
+    <t>105846</t>
+  </si>
+  <si>
+    <t>110357</t>
+  </si>
+  <si>
+    <t>111243</t>
+  </si>
+  <si>
+    <t>112435</t>
+  </si>
+  <si>
+    <t>112436</t>
+  </si>
+  <si>
+    <t>112601</t>
+  </si>
+  <si>
+    <t>112602</t>
+  </si>
+  <si>
+    <t>113151</t>
+  </si>
+  <si>
+    <t>154935</t>
+  </si>
+  <si>
+    <t>154936</t>
+  </si>
+  <si>
+    <t>162126</t>
+  </si>
+  <si>
+    <t>162127</t>
+  </si>
+  <si>
+    <t>162500</t>
   </si>
 </sst>
 </file>
@@ -848,7 +908,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,25 +972,25 @@
         <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E2" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I2" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>14</v>
@@ -954,7 +1014,7 @@
       <formula1>"UAT,E2E"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{522E0E79-AC07-422F-B8D2-DC41E42871EC}">
-      <formula1>"approvalForm,repaymentForm,realizationForm,validationApprovalFile,validationRealizationFile"</formula1>
+      <formula1>"approvalForm,realizationForm,validationApprovalFile,validationRealizationFile"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2197,13 +2257,13 @@
         <v>48</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E57" s="13" t="s">
         <v>48</v>
       </c>
       <c r="F57" s="13" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2212,33 +2272,33 @@
     <row r="61" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="B62" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="C62" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D62" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E62" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="F62" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B63" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C63" s="5" t="s">
         <v>84</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F63" s="5" t="s">
         <v>84</v>
@@ -2246,30 +2306,30 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B64" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="65" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>